<commit_message>
Feat : Add New Skills
- Add ShadowStrike

- Add Evade

- Fix Acting&Stealth Logic

- Modify Impulse System
(Use Unreal Curve)

- Add CurveManager
</commit_message>
<xml_diff>
--- a/GameData/SLCharacterSkillDatas.xlsx
+++ b/GameData/SLCharacterSkillDatas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongchan\Documents\Unreal Projects\SekiroLike\UnrealSoloProject\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F3196E-F7A2-465A-B188-6E444AAAC98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6396531-6A8A-465D-8498-AD6B534BDC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="23880" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,11 +39,11 @@
     <t>AttackRadius</t>
   </si>
   <si>
-    <t>A</t>
+    <t>RushAttack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RushAttack</t>
+    <t>ShadowStrike</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -372,7 +372,7 @@
   <dimension ref="B2:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -399,7 +399,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0.6</v>
@@ -413,16 +413,16 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E4">
-        <v>70</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat : Add Effect & TargetSystem
- Add Effect
 * ThrowingKnife
 * Combo Attack
 * Rush Attack
 * Shadow Strike
 * Evade
 * Steath Mode

 - MP interlocking

- TargetSystem & LockOn Camera
 * LockOn to Target
 * Can Toggle
 * Player -> Target : LineTracing
 * Change target to Mouse Input
</commit_message>
<xml_diff>
--- a/GameData/SLCharacterSkillDatas.xlsx
+++ b/GameData/SLCharacterSkillDatas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dongchan\Documents\Unreal Projects\SekiroLike\UnrealSoloProject\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6396531-6A8A-465D-8498-AD6B534BDC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E6E2B3-2187-4CE0-8330-8C3CD6C8BAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="23880" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -44,6 +44,17 @@
   </si>
   <si>
     <t>ShadowStrike</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThrowKnife</t>
+  </si>
+  <si>
+    <t>Mp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Evade</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -369,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E4"/>
+  <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -383,7 +394,7 @@
     <col min="5" max="5" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -396,8 +407,11 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -410,8 +424,11 @@
       <c r="E3">
         <v>120</v>
       </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -423,6 +440,43 @@
       </c>
       <c r="E4">
         <v>120</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>